<commit_message>
Added CO2 emission for cruises
</commit_message>
<xml_diff>
--- a/data/iAtlantic_cruises/2019_PS120_leg1_participants.xlsx
+++ b/data/iAtlantic_cruises/2019_PS120_leg1_participants.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sa07kb\Projects\iAtlantic\Subprojects\CO2_footprint\data\iAtlantic_cruises\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C697F39-E1B4-4B94-AB86-940D72FC74F2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DE1E3005-696C-43B1-A58B-C81DD72C741F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="795" windowWidth="19200" windowHeight="10200" xr2:uid="{129D3273-36BB-4451-8151-5163F1722E58}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{129D3273-36BB-4451-8151-5163F1722E58}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="2019_PS120_leg1_participants" sheetId="2" r:id="rId2"/>
+    <sheet name="2019_PS120_leg1_participants_fr" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="15">
   <si>
     <t>cruise</t>
   </si>
@@ -73,6 +75,12 @@
   </si>
   <si>
     <t>Germany</t>
+  </si>
+  <si>
+    <t>Falkland Islands</t>
+  </si>
+  <si>
+    <t>Gran Canaria</t>
   </si>
 </sst>
 </file>
@@ -427,8 +435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06CBFB0F-A008-4715-99CA-D3AD37AC3BEB}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,4 +527,115 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A26F6AB3-01F8-44DB-B92D-F436CEA8730A}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28B13D9D-1D7E-4EBC-BB0E-6ED1C05FE5CB}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>